<commit_message>
with settings , gate pass etc
</commit_message>
<xml_diff>
--- a/scheduled_reports/ticket_cost_report.xlsx
+++ b/scheduled_reports/ticket_cost_report.xlsx
@@ -13,10 +13,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Reference No</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Created At</t>
+  </si>
+  <si>
+    <t>Service Cost</t>
+  </si>
+  <si>
+    <t>REF-20250731-001</t>
+  </si>
+  <si>
+    <t>REF-20250731-002</t>
+  </si>
+  <si>
+    <t>REF-20250731-003</t>
+  </si>
+  <si>
+    <t>CRESTANKS LIMITED</t>
+  </si>
+  <si>
+    <t>KYAGALANYI COFFEE LIMITED</t>
+  </si>
+  <si>
+    <t>UGANDA REVENUE AUTHORITY</t>
+  </si>
+  <si>
+    <t>2025-07-30</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +86,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +404,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>